<commit_message>
fix: change plan template
</commit_message>
<xml_diff>
--- a/assets/template_excel/Template Upload Daily Plan.xlsx
+++ b/assets/template_excel/Template Upload Daily Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riko_Tan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Programming\Yanmar\yanmar_app\assets\template_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA376550-1505-4E6F-BDE3-F512C92F4153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E54944-BD6A-4409-91A2-EB0840EED1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D7FB3311-D43C-42F2-AB52-C1807F123975}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -124,9 +124,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,12 +464,12 @@
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -500,11 +497,11 @@
       <c r="I1" s="1">
         <v>7</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -516,7 +513,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -528,7 +525,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -540,7 +537,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -552,7 +549,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -564,7 +561,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -576,7 +573,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -588,7 +585,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -600,7 +597,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -612,7 +609,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -634,17 +631,17 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -655,7 +652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -666,7 +663,7 @@
         <v>0.35416666666666669</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -677,7 +674,7 @@
         <v>0.39583333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -688,7 +685,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -696,51 +693,51 @@
         <v>0.4375</v>
       </c>
       <c r="C5" s="2">
-        <v>0.47916666666666669</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.48958333333333331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>0.54166666666666663</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="C6" s="2">
-        <v>0.58333333333333337</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="C7" s="2">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.60416666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>0.625</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="C8" s="2">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+        <v>0.64583333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.66666666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C9" s="2">
-        <v>0.70833333333333337</v>
+        <v>0.6875</v>
       </c>
     </row>
   </sheetData>
@@ -760,12 +757,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3">
       <c r="B2" t="s">
         <v>5</v>
       </c>

</xml_diff>